<commit_message>
Added support for resw files for mac version
</commit_message>
<xml_diff>
--- a/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.fr-FR.resx.xlsx
+++ b/src/Samples/MultilingualExtensionSampleConsoleApp/Resources/AppResources.fr-FR.resx.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -38,13 +38,61 @@
     <t xml:space="preserve">Enter_Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter email please</t>
+    <t xml:space="preserve">Enter email please!</t>
   </si>
   <si>
     <t xml:space="preserve">Entrez e-mail s’il vous plaît</t>
   </si>
   <si>
-    <t xml:space="preserve">New</t>
+    <t xml:space="preserve">Enter_Email_To_Be_The_Next_User_To_Be_Able_To_Login_To_The_Best_Office_System_In_The_World</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrez e-mail s’il vous plaît!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mot de passe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accueil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press_Any_Key_To_Exit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press any key to exit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appuyez sur n’importe quelle clé pour sortir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oiseau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vache</t>
   </si>
 </sst>
 </file>
@@ -135,9 +183,129 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="E3"/>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>